<commit_message>
update docs and cleanup
</commit_message>
<xml_diff>
--- a/vignettes/articles/metadata_template.xlsx
+++ b/vignettes/articles/metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1679488-CED5-304E-8E14-5C24EE10EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D1A804-2E7F-9A42-AF65-F45D8BC369B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -763,6 +763,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{0B3BC74F-042E-D940-8ED2-CE367BFE1CE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Either 'linear' or 'quadratic'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{1BE932C9-295D-1049-B7C7-2AA12E6D503E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Either '1/x', '1/x2' or 'none'</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -927,7 +955,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>analysis_id</t>
   </si>
@@ -1142,6 +1170,12 @@
   </si>
   <si>
     <t>chem_formula</t>
+  </si>
+  <si>
+    <t>Curve_Fit_Model</t>
+  </si>
+  <si>
+    <t>Curve_Fit_Weighting</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2377,7 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2678,10 +2712,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2694,10 +2728,11 @@
     <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2735,6 +2770,12 @@
         <v>14</v>
       </c>
       <c r="M1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>